<commit_message>
added method notes, started pilot paradigm code
</commit_message>
<xml_diff>
--- a/stmuli/genetic_180_rand_jitter_run45.xlsx
+++ b/stmuli/genetic_180_rand_jitter_run45.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499EBBE-D681-45AD-90C7-333A614F9763}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3942A4-176F-41B4-9E9A-1697CADE0E33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1study_jitter" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="v2study_jitter" sheetId="2" r:id="rId3"/>
     <sheet name="v2test_jitter" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,6 +21,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -645,7 +646,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="608">
+  <dxfs count="437">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4992,1707 +4993,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -6971,8 +5271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P451"/>
   <sheetViews>
-    <sheetView topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="D445" sqref="D445"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -47083,7 +45383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673A43C1-0202-4750-9CCA-49EE1BC11C37}">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E137" sqref="E137:H181"/>
     </sheetView>
   </sheetViews>

</xml_diff>